<commit_message>
add original mend for synstory
</commit_message>
<xml_diff>
--- a/synstory_exp_out/4K_heavy_noshare_midupper3/syn_story/mend_eval_loss=clm_input=seen_n=100_prompt=no_w-gen_wo-icl_4K_test_ood-question.xlsx
+++ b/synstory_exp_out/4K_heavy_noshare_midupper3/syn_story/mend_eval_loss=clm_input=seen_n=100_prompt=no_w-gen_wo-icl_4K_test_ood-question.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I253"/>
+  <dimension ref="A1:J253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,12 +479,15 @@
           <t>predicted_answer</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>llm_accuracy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -524,12 +527,13 @@
           <t>George Bernard Shaw</t>
         </is>
       </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A3" t="n">
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -569,12 +573,13 @@
           <t>Asghar Farhadi</t>
         </is>
       </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A4" t="n">
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -614,12 +619,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A5" t="n">
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -659,12 +665,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A6" t="n">
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -704,12 +711,13 @@
           <t>9/11</t>
         </is>
       </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A7" t="n">
+        <v>2</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -749,12 +757,13 @@
           <t>1969</t>
         </is>
       </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A8" t="n">
+        <v>2</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -794,12 +803,13 @@
           <t>1789</t>
         </is>
       </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A9" t="n">
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -839,12 +849,13 @@
           <t>1799</t>
         </is>
       </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A10" t="n">
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -884,12 +895,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A11" t="n">
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -929,12 +941,13 @@
           <t>Protestantism</t>
         </is>
       </c>
+      <c r="J11" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A12" t="n">
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -974,12 +987,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A13" t="n">
+        <v>4</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1019,12 +1033,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A14" t="n">
+        <v>5</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1064,12 +1079,13 @@
           <t>Pablo Picasso</t>
         </is>
       </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A15" t="n">
+        <v>5</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1109,12 +1125,13 @@
           <t>Cormac McCarthy</t>
         </is>
       </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A16" t="n">
+        <v>6</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1154,12 +1171,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A17" t="n">
+        <v>6</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1199,12 +1217,13 @@
           <t>1969</t>
         </is>
       </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A18" t="n">
+        <v>6</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1244,12 +1263,13 @@
           <t>1789</t>
         </is>
       </c>
+      <c r="J18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A19" t="n">
+        <v>6</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1289,12 +1309,13 @@
           <t>1648</t>
         </is>
       </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A20" t="n">
+        <v>7</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1334,12 +1355,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A21" t="n">
+        <v>7</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1379,12 +1401,13 @@
           <t>Cyrillic</t>
         </is>
       </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A22" t="n">
+        <v>8</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1424,12 +1447,13 @@
           <t>2010</t>
         </is>
       </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A23" t="n">
+        <v>8</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1469,12 +1493,13 @@
           <t>2009</t>
         </is>
       </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A24" t="n">
+        <v>8</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1514,12 +1539,13 @@
           <t>1642 to 1651</t>
         </is>
       </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A25" t="n">
+        <v>8</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1559,12 +1585,13 @@
           <t>1651</t>
         </is>
       </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A26" t="n">
+        <v>9</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1604,12 +1631,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A27" t="n">
+        <v>9</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1649,12 +1677,13 @@
           <t>Protestantism</t>
         </is>
       </c>
+      <c r="J27" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A28" t="n">
+        <v>10</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1694,12 +1723,13 @@
           <t>Stephen King</t>
         </is>
       </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A29" t="n">
+        <v>10</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1739,12 +1769,13 @@
           <t>Cormac McCarthy</t>
         </is>
       </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A30" t="n">
+        <v>11</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1784,12 +1815,13 @@
           <t>1984</t>
         </is>
       </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A31" t="n">
+        <v>11</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1829,12 +1861,13 @@
           <t>1977</t>
         </is>
       </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A32" t="n">
+        <v>11</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1874,12 +1907,13 @@
           <t>1789</t>
         </is>
       </c>
+      <c r="J32" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A33" t="n">
+        <v>11</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1919,12 +1953,13 @@
           <t>1956</t>
         </is>
       </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A34" t="n">
+        <v>12</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1964,12 +1999,13 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A35" t="n">
+        <v>12</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2009,12 +2045,13 @@
           <t>Tropical and subtropical oceans</t>
         </is>
       </c>
+      <c r="J35" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="A36" t="n">
+        <v>13</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -2054,12 +2091,13 @@
           <t>Cyrillic</t>
         </is>
       </c>
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="A37" t="n">
+        <v>13</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -2099,12 +2137,13 @@
           <t>Cyrillic</t>
         </is>
       </c>
+      <c r="J37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="A38" t="n">
+        <v>14</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -2144,12 +2183,13 @@
           <t>Andy Warhol</t>
         </is>
       </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="A39" t="n">
+        <v>14</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -2189,12 +2229,13 @@
           <t>Guillermo del Toro</t>
         </is>
       </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A40" t="n">
+        <v>15</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -2234,12 +2275,13 @@
           <t>1999</t>
         </is>
       </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A41" t="n">
+        <v>15</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -2279,12 +2321,13 @@
           <t>2010</t>
         </is>
       </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A42" t="n">
+        <v>15</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -2324,12 +2367,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J42" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A43" t="n">
+        <v>15</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -2369,12 +2413,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="A44" t="n">
+        <v>16</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2414,12 +2459,13 @@
           <t>David Cameron</t>
         </is>
       </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="A45" t="n">
+        <v>16</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2459,12 +2505,13 @@
           <t>Asghar Farhadi</t>
         </is>
       </c>
+      <c r="J45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="A46" t="n">
+        <v>17</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2504,12 +2551,13 @@
           <t>Brazil</t>
         </is>
       </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="A47" t="n">
+        <v>17</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2549,12 +2597,13 @@
           <t>Tropical and subtropical regions of the Americas, Africa, and Asia</t>
         </is>
       </c>
+      <c r="J47" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="A48" t="n">
+        <v>18</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -2594,12 +2643,13 @@
           <t>Tamilalam</t>
         </is>
       </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="A49" t="n">
+        <v>18</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -2639,12 +2689,13 @@
           <t>Sinhalese script</t>
         </is>
       </c>
+      <c r="J49" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="A50" t="n">
+        <v>19</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -2684,12 +2735,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="A51" t="n">
+        <v>19</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2729,12 +2781,13 @@
           <t>Tropical and subtropical oceans</t>
         </is>
       </c>
+      <c r="J51" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="A52" t="n">
+        <v>20</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -2774,12 +2827,13 @@
           <t>Hawaii</t>
         </is>
       </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="A53" t="n">
+        <v>20</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -2819,12 +2873,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="A54" t="n">
+        <v>21</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -2864,12 +2919,13 @@
           <t>1994</t>
         </is>
       </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="A55" t="n">
+        <v>21</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2909,12 +2965,13 @@
           <t>2009</t>
         </is>
       </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="A56" t="n">
+        <v>21</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2954,12 +3011,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J56" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="A57" t="n">
+        <v>21</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2999,12 +3057,13 @@
           <t>1648</t>
         </is>
       </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="A58" t="n">
+        <v>22</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -3044,12 +3103,13 @@
           <t>2009</t>
         </is>
       </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="A59" t="n">
+        <v>22</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -3089,12 +3149,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="A60" t="n">
+        <v>22</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -3134,12 +3195,13 @@
           <t>16th century</t>
         </is>
       </c>
+      <c r="J60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="A61" t="n">
+        <v>22</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -3179,12 +3241,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="A62" t="n">
+        <v>23</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -3224,12 +3287,13 @@
           <t>Christian</t>
         </is>
       </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="A63" t="n">
+        <v>23</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -3269,12 +3333,13 @@
           <t>Shia Islam</t>
         </is>
       </c>
+      <c r="J63" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="A64" t="n">
+        <v>24</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -3314,12 +3379,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J64" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="A65" t="n">
+        <v>24</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -3359,12 +3425,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A66" t="n">
+        <v>25</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -3404,12 +3471,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A67" t="n">
+        <v>25</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -3449,12 +3517,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A68" t="n">
+        <v>25</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -3494,12 +3563,13 @@
           <t>September 11, 2001</t>
         </is>
       </c>
+      <c r="J68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A69" t="n">
+        <v>25</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -3539,12 +3609,13 @@
           <t>1799</t>
         </is>
       </c>
+      <c r="J69" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="A70" t="n">
+        <v>26</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -3584,12 +3655,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="A71" t="n">
+        <v>26</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -3629,12 +3701,13 @@
           <t>Cyrillic</t>
         </is>
       </c>
+      <c r="J71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="A72" t="n">
+        <v>27</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -3674,12 +3747,13 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="A73" t="n">
+        <v>27</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -3719,12 +3793,13 @@
           <t>China</t>
         </is>
       </c>
+      <c r="J73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="A74" t="n">
+        <v>28</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -3764,12 +3839,13 @@
           <t>1914</t>
         </is>
       </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="A75" t="n">
+        <v>28</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -3809,12 +3885,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="A76" t="n">
+        <v>28</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -3854,12 +3931,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J76" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="A77" t="n">
+        <v>28</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -3899,12 +3977,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="A78" t="n">
+        <v>29</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -3944,12 +4023,13 @@
           <t>Brazil</t>
         </is>
       </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="A79" t="n">
+        <v>29</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -3989,12 +4069,13 @@
           <t>Tropical and subtropical regions of the Americas, Africa, and Asia</t>
         </is>
       </c>
+      <c r="J79" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="A80" t="n">
+        <v>30</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -4034,12 +4115,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="A81" t="n">
+        <v>30</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -4079,12 +4161,13 @@
           <t>2001</t>
         </is>
       </c>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="A82" t="n">
+        <v>30</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -4124,12 +4207,13 @@
           <t>1955</t>
         </is>
       </c>
+      <c r="J82" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="A83" t="n">
+        <v>30</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -4169,12 +4253,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="A84" t="n">
+        <v>31</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -4214,12 +4299,13 @@
           <t>Neil Gaiman</t>
         </is>
       </c>
+      <c r="J84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="A85" t="n">
+        <v>31</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -4259,12 +4345,13 @@
           <t>Hayao Miyazaki</t>
         </is>
       </c>
+      <c r="J85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="A86" t="n">
+        <v>32</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -4304,12 +4391,13 @@
           <t>1971</t>
         </is>
       </c>
+      <c r="J86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="A87" t="n">
+        <v>32</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -4349,12 +4437,13 @@
           <t>2001</t>
         </is>
       </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="A88" t="n">
+        <v>32</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -4394,12 +4483,13 @@
           <t>16th century</t>
         </is>
       </c>
+      <c r="J88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="A89" t="n">
+        <v>32</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -4439,12 +4529,13 @@
           <t>1648</t>
         </is>
       </c>
+      <c r="J89" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="A90" t="n">
+        <v>33</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -4484,12 +4575,13 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="J90" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="A91" t="n">
+        <v>33</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -4529,12 +4621,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="A92" t="n">
+        <v>34</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -4574,12 +4667,13 @@
           <t>South America</t>
         </is>
       </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="A93" t="n">
+        <v>34</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -4619,12 +4713,13 @@
           <t>Tropical and subtropical oceans</t>
         </is>
       </c>
+      <c r="J93" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="A94" t="n">
+        <v>35</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -4664,12 +4759,13 @@
           <t>1919</t>
         </is>
       </c>
+      <c r="J94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="A95" t="n">
+        <v>35</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -4709,12 +4805,13 @@
           <t>1972</t>
         </is>
       </c>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="A96" t="n">
+        <v>35</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -4754,12 +4851,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J96" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="A97" t="n">
+        <v>35</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -4799,12 +4897,13 @@
           <t>2001</t>
         </is>
       </c>
+      <c r="J97" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="A98" t="n">
+        <v>36</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -4844,12 +4943,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J98" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="A99" t="n">
+        <v>36</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -4889,12 +4989,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J99" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+      <c r="A100" t="n">
+        <v>37</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -4934,12 +5035,13 @@
           <t>Steve Jobs</t>
         </is>
       </c>
+      <c r="J100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+      <c r="A101" t="n">
+        <v>37</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -4979,12 +5081,13 @@
           <t>Guillermo del Toro</t>
         </is>
       </c>
+      <c r="J101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="A102" t="n">
+        <v>38</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -5024,12 +5127,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="A103" t="n">
+        <v>38</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -5069,12 +5173,13 @@
           <t>Northern, central, and eastern Africa</t>
         </is>
       </c>
+      <c r="J103" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="A104" t="n">
+        <v>39</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -5114,12 +5219,13 @@
           <t>9/11</t>
         </is>
       </c>
+      <c r="J104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="A105" t="n">
+        <v>39</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -5159,12 +5265,13 @@
           <t>2014</t>
         </is>
       </c>
+      <c r="J105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="A106" t="n">
+        <v>39</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -5204,12 +5311,13 @@
           <t>1642 to 1651</t>
         </is>
       </c>
+      <c r="J106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="A107" t="n">
+        <v>39</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -5249,12 +5357,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="A108" t="n">
+        <v>40</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -5294,12 +5403,13 @@
           <t>Sinhala and Tamil</t>
         </is>
       </c>
+      <c r="J108" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="A109" t="n">
+        <v>40</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -5339,12 +5449,13 @@
           <t>Sinhala script</t>
         </is>
       </c>
+      <c r="J109" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+      <c r="A110" t="n">
+        <v>41</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -5384,12 +5495,13 @@
           <t>The Philippines</t>
         </is>
       </c>
+      <c r="J110" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+      <c r="A111" t="n">
+        <v>41</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -5429,12 +5541,13 @@
           <t>Tropical and subtropical waters</t>
         </is>
       </c>
+      <c r="J111" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="A112" t="n">
+        <v>42</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -5474,12 +5587,13 @@
           <t>Steve Jobs</t>
         </is>
       </c>
+      <c r="J112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="A113" t="n">
+        <v>42</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -5519,12 +5633,13 @@
           <t>Cormac McCarthy</t>
         </is>
       </c>
+      <c r="J113" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="A114" t="n">
+        <v>43</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -5564,12 +5679,13 @@
           <t>1928</t>
         </is>
       </c>
+      <c r="J114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="A115" t="n">
+        <v>43</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -5609,12 +5725,13 @@
           <t>2007</t>
         </is>
       </c>
+      <c r="J115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="A116" t="n">
+        <v>43</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -5654,12 +5771,13 @@
           <t>1803 to 1815</t>
         </is>
       </c>
+      <c r="J116" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="A117" t="n">
+        <v>43</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -5699,12 +5817,13 @@
           <t>1648</t>
         </is>
       </c>
+      <c r="J117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="A118" t="n">
+        <v>44</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -5744,12 +5863,13 @@
           <t>Christian</t>
         </is>
       </c>
+      <c r="J118" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="A119" t="n">
+        <v>44</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -5789,12 +5909,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J119" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="A120" t="n">
+        <v>45</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -5834,12 +5955,13 @@
           <t>New York City, New York, USA</t>
         </is>
       </c>
+      <c r="J120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="A121" t="n">
+        <v>45</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -5879,12 +6001,13 @@
           <t>Burbank, California, USA</t>
         </is>
       </c>
+      <c r="J121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
+      <c r="A122" t="n">
+        <v>46</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -5924,12 +6047,13 @@
           <t>Steve Jobs</t>
         </is>
       </c>
+      <c r="J122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
+      <c r="A123" t="n">
+        <v>46</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -5969,12 +6093,13 @@
           <t>Asghar Farhadi</t>
         </is>
       </c>
+      <c r="J123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="A124" t="n">
+        <v>47</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -6014,12 +6139,13 @@
           <t>Christian</t>
         </is>
       </c>
+      <c r="J124" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="A125" t="n">
+        <v>47</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -6059,12 +6185,13 @@
           <t>Protestantism</t>
         </is>
       </c>
+      <c r="J125" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="A126" t="n">
+        <v>48</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -6104,12 +6231,13 @@
           <t>Brazil</t>
         </is>
       </c>
+      <c r="J126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="A127" t="n">
+        <v>48</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -6149,12 +6277,13 @@
           <t>Tropical and subtropical waters of the Pacific Ocean</t>
         </is>
       </c>
+      <c r="J127" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="A128" t="n">
+        <v>49</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -6194,12 +6323,13 @@
           <t>Christian</t>
         </is>
       </c>
+      <c r="J128" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="A129" t="n">
+        <v>49</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -6239,12 +6369,13 @@
           <t>Protestantism</t>
         </is>
       </c>
+      <c r="J129" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="A130" t="n">
+        <v>50</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -6284,12 +6415,13 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="A131" t="n">
+        <v>50</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -6329,12 +6461,13 @@
           <t>Tropical and subtropical waters of the Pacific Ocean</t>
         </is>
       </c>
+      <c r="J131" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
+      <c r="A132" t="n">
+        <v>51</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -6374,12 +6507,13 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="J132" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
+      <c r="A133" t="n">
+        <v>51</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -6419,12 +6553,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J133" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
+      <c r="A134" t="n">
+        <v>52</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -6464,12 +6599,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J134" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
+      <c r="A135" t="n">
+        <v>52</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -6509,12 +6645,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J135" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
+      <c r="A136" t="n">
+        <v>53</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -6554,12 +6691,13 @@
           <t>1 January 2000</t>
         </is>
       </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
+      <c r="A137" t="n">
+        <v>53</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -6599,12 +6737,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J137" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
+      <c r="A138" t="n">
+        <v>53</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -6644,12 +6783,13 @@
           <t>December 16, 1773</t>
         </is>
       </c>
+      <c r="J138" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
+      <c r="A139" t="n">
+        <v>53</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -6689,12 +6829,13 @@
           <t>1651</t>
         </is>
       </c>
+      <c r="J139" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
+      <c r="A140" t="n">
+        <v>54</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -6734,12 +6875,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
+      <c r="A141" t="n">
+        <v>54</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -6779,12 +6921,13 @@
           <t>1969</t>
         </is>
       </c>
+      <c r="J141" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
+      <c r="A142" t="n">
+        <v>54</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -6824,12 +6967,13 @@
           <t>1791 to 1804</t>
         </is>
       </c>
+      <c r="J142" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
+      <c r="A143" t="n">
+        <v>54</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -6869,12 +7013,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J143" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
+      <c r="A144" t="n">
+        <v>55</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -6914,12 +7059,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J144" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
+      <c r="A145" t="n">
+        <v>55</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -6959,12 +7105,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J145" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
+      <c r="A146" t="n">
+        <v>56</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -7004,12 +7151,13 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="J146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
+      <c r="A147" t="n">
+        <v>56</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -7049,12 +7197,13 @@
           <t>Central and South America</t>
         </is>
       </c>
+      <c r="J147" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="A148" t="n">
+        <v>57</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -7094,12 +7243,13 @@
           <t>Devanagari</t>
         </is>
       </c>
+      <c r="J148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="A149" t="n">
+        <v>57</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -7139,12 +7289,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J149" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="A150" t="n">
+        <v>58</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -7184,12 +7335,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J150" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="A151" t="n">
+        <v>58</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -7229,12 +7381,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J151" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="A152" t="n">
+        <v>59</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -7274,12 +7427,13 @@
           <t>1 January 2009</t>
         </is>
       </c>
+      <c r="J152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="A153" t="n">
+        <v>59</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -7319,12 +7473,13 @@
           <t>2007</t>
         </is>
       </c>
+      <c r="J153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="A154" t="n">
+        <v>59</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -7364,12 +7519,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J154" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="A155" t="n">
+        <v>59</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -7409,12 +7565,13 @@
           <t>1815</t>
         </is>
       </c>
+      <c r="J155" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="A156" t="n">
+        <v>60</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -7454,12 +7611,13 @@
           <t>Christian</t>
         </is>
       </c>
+      <c r="J156" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="A157" t="n">
+        <v>60</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -7499,12 +7657,13 @@
           <t>Shia Islam</t>
         </is>
       </c>
+      <c r="J157" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
+      <c r="A158" t="n">
+        <v>61</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -7544,12 +7703,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J158" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
+      <c r="A159" t="n">
+        <v>61</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -7589,12 +7749,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J159" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+      <c r="A160" t="n">
+        <v>62</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -7634,12 +7795,13 @@
           <t>Brazil</t>
         </is>
       </c>
+      <c r="J160" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+      <c r="A161" t="n">
+        <v>62</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -7679,12 +7841,13 @@
           <t>Tropical and subtropical regions of the Americas, Africa, and Asia</t>
         </is>
       </c>
+      <c r="J161" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
+      <c r="A162" t="n">
+        <v>63</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -7724,12 +7887,13 @@
           <t>Brazil</t>
         </is>
       </c>
+      <c r="J162" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
+      <c r="A163" t="n">
+        <v>63</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -7769,12 +7933,13 @@
           <t>Tropical and subtropical regions of the Americas, Africa, and Asia</t>
         </is>
       </c>
+      <c r="J163" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="A164" t="n">
+        <v>64</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -7814,12 +7979,13 @@
           <t>1991</t>
         </is>
       </c>
+      <c r="J164" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="A165" t="n">
+        <v>64</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -7859,12 +8025,13 @@
           <t>2009</t>
         </is>
       </c>
+      <c r="J165" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="A166" t="n">
+        <v>64</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -7904,12 +8071,13 @@
           <t>1803 to 1815</t>
         </is>
       </c>
+      <c r="J166" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="A167" t="n">
+        <v>64</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -7949,12 +8117,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J167" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="A168" t="n">
+        <v>65</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -7994,12 +8163,13 @@
           <t>Brazil</t>
         </is>
       </c>
+      <c r="J168" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="A169" t="n">
+        <v>65</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -8039,12 +8209,13 @@
           <t>Tropical and subtropical regions of the Americas, Africa, and Asia</t>
         </is>
       </c>
+      <c r="J169" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+      <c r="A170" t="n">
+        <v>66</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -8084,12 +8255,13 @@
           <t>1858</t>
         </is>
       </c>
+      <c r="J170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+      <c r="A171" t="n">
+        <v>66</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -8129,12 +8301,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J171" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+      <c r="A172" t="n">
+        <v>66</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -8174,12 +8347,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J172" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+      <c r="A173" t="n">
+        <v>66</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -8219,12 +8393,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J173" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>67</t>
-        </is>
+      <c r="A174" t="n">
+        <v>67</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -8264,12 +8439,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J174" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>67</t>
-        </is>
+      <c r="A175" t="n">
+        <v>67</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -8309,12 +8485,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J175" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+      <c r="A176" t="n">
+        <v>68</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -8354,12 +8531,13 @@
           <t>Afrikaans</t>
         </is>
       </c>
+      <c r="J176" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+      <c r="A177" t="n">
+        <v>68</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -8399,12 +8577,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J177" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+      <c r="A178" t="n">
+        <v>69</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -8444,12 +8623,13 @@
           <t>2014</t>
         </is>
       </c>
+      <c r="J178" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+      <c r="A179" t="n">
+        <v>69</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -8489,12 +8669,13 @@
           <t>2009</t>
         </is>
       </c>
+      <c r="J179" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+      <c r="A180" t="n">
+        <v>69</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -8534,12 +8715,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J180" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+      <c r="A181" t="n">
+        <v>69</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -8579,12 +8761,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J181" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+      <c r="A182" t="n">
+        <v>70</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -8624,12 +8807,13 @@
           <t>Islam</t>
         </is>
       </c>
+      <c r="J182" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+      <c r="A183" t="n">
+        <v>70</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -8669,12 +8853,13 @@
           <t>Shia Islam</t>
         </is>
       </c>
+      <c r="J183" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="A184" t="n">
+        <v>71</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -8714,12 +8899,13 @@
           <t>9/11</t>
         </is>
       </c>
+      <c r="J184" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="A185" t="n">
+        <v>71</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
@@ -8759,12 +8945,13 @@
           <t>2001</t>
         </is>
       </c>
+      <c r="J185" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="A186" t="n">
+        <v>71</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
@@ -8804,12 +8991,13 @@
           <t>16th century</t>
         </is>
       </c>
+      <c r="J186" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="A187" t="n">
+        <v>71</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
@@ -8849,12 +9037,13 @@
           <t>1648</t>
         </is>
       </c>
+      <c r="J187" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>72</t>
-        </is>
+      <c r="A188" t="n">
+        <v>72</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -8894,12 +9083,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J188" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>72</t>
-        </is>
+      <c r="A189" t="n">
+        <v>72</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
@@ -8939,12 +9129,13 @@
           <t>Sinhalese script</t>
         </is>
       </c>
+      <c r="J189" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="A190" t="n">
+        <v>73</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -8984,12 +9175,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J190" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="A191" t="n">
+        <v>73</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -9029,12 +9221,13 @@
           <t>Sinhalese script</t>
         </is>
       </c>
+      <c r="J191" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="A192" t="n">
+        <v>74</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
@@ -9074,12 +9267,13 @@
           <t>1914</t>
         </is>
       </c>
+      <c r="J192" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="A193" t="n">
+        <v>74</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
@@ -9119,12 +9313,13 @@
           <t>2010</t>
         </is>
       </c>
+      <c r="J193" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="194">
-      <c r="A194" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="A194" t="n">
+        <v>74</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
@@ -9164,12 +9359,13 @@
           <t>1066</t>
         </is>
       </c>
+      <c r="J194" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="A195" t="n">
+        <v>74</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
@@ -9209,12 +9405,13 @@
           <t>1804</t>
         </is>
       </c>
+      <c r="J195" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+      <c r="A196" t="n">
+        <v>75</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
@@ -9254,12 +9451,13 @@
           <t>Mikhail Gorbachev</t>
         </is>
       </c>
+      <c r="J196" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+      <c r="A197" t="n">
+        <v>75</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
@@ -9299,12 +9497,13 @@
           <t>Cormac McCarthy</t>
         </is>
       </c>
+      <c r="J197" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
+      <c r="A198" t="n">
+        <v>76</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
@@ -9344,12 +9543,13 @@
           <t>2009</t>
         </is>
       </c>
+      <c r="J198" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
+      <c r="A199" t="n">
+        <v>76</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
@@ -9389,12 +9589,13 @@
           <t>2008</t>
         </is>
       </c>
+      <c r="J199" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
+      <c r="A200" t="n">
+        <v>76</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
@@ -9434,12 +9635,13 @@
           <t>December 16, 1773</t>
         </is>
       </c>
+      <c r="J200" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
+      <c r="A201" t="n">
+        <v>76</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
@@ -9479,12 +9681,13 @@
           <t>1648</t>
         </is>
       </c>
+      <c r="J201" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+      <c r="A202" t="n">
+        <v>77</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
@@ -9524,12 +9727,13 @@
           <t>Neil Gaiman</t>
         </is>
       </c>
+      <c r="J202" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+      <c r="A203" t="n">
+        <v>77</v>
       </c>
       <c r="B203" t="inlineStr">
         <is>
@@ -9569,12 +9773,13 @@
           <t>Guillermo del Toro</t>
         </is>
       </c>
+      <c r="J203" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
+      <c r="A204" t="n">
+        <v>78</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
@@ -9614,12 +9819,13 @@
           <t>Christian</t>
         </is>
       </c>
+      <c r="J204" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
+      <c r="A205" t="n">
+        <v>78</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
@@ -9659,12 +9865,13 @@
           <t>Shia Islam</t>
         </is>
       </c>
+      <c r="J205" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="A206" t="n">
+        <v>79</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
@@ -9704,12 +9911,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J206" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="A207" t="n">
+        <v>79</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
@@ -9749,12 +9957,13 @@
           <t>Protestantism</t>
         </is>
       </c>
+      <c r="J207" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="A208" t="n">
+        <v>80</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
@@ -9794,12 +10003,13 @@
           <t>1969</t>
         </is>
       </c>
+      <c r="J208" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="A209" t="n">
+        <v>80</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
@@ -9839,12 +10049,13 @@
           <t>1994</t>
         </is>
       </c>
+      <c r="J209" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="A210" t="n">
+        <v>80</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
@@ -9884,12 +10095,13 @@
           <t>1803 to 1815</t>
         </is>
       </c>
+      <c r="J210" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="A211" t="n">
+        <v>80</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
@@ -9929,12 +10141,13 @@
           <t>1815</t>
         </is>
       </c>
+      <c r="J211" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
+      <c r="A212" t="n">
+        <v>81</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
@@ -9974,12 +10187,13 @@
           <t>1789</t>
         </is>
       </c>
+      <c r="J212" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
+      <c r="A213" t="n">
+        <v>81</v>
       </c>
       <c r="B213" t="inlineStr">
         <is>
@@ -10019,12 +10233,13 @@
           <t>1972</t>
         </is>
       </c>
+      <c r="J213" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
-      <c r="A214" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
+      <c r="A214" t="n">
+        <v>81</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
@@ -10064,12 +10279,13 @@
           <t>December 16, 1773</t>
         </is>
       </c>
+      <c r="J214" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
+      <c r="A215" t="n">
+        <v>81</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
@@ -10109,12 +10325,13 @@
           <t>1773</t>
         </is>
       </c>
+      <c r="J215" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t>82</t>
-        </is>
+      <c r="A216" t="n">
+        <v>82</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
@@ -10154,12 +10371,13 @@
           <t>Devanagari</t>
         </is>
       </c>
+      <c r="J216" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>82</t>
-        </is>
+      <c r="A217" t="n">
+        <v>82</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
@@ -10199,12 +10417,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J217" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
+      <c r="A218" t="n">
+        <v>83</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
@@ -10244,12 +10463,13 @@
           <t>Hawaii</t>
         </is>
       </c>
+      <c r="J218" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
+      <c r="A219" t="n">
+        <v>83</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
@@ -10289,12 +10509,13 @@
           <t>Central and South America</t>
         </is>
       </c>
+      <c r="J219" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr">
-        <is>
-          <t>84</t>
-        </is>
+      <c r="A220" t="n">
+        <v>84</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
@@ -10334,12 +10555,13 @@
           <t>Madagascar</t>
         </is>
       </c>
+      <c r="J220" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
-      <c r="A221" t="inlineStr">
-        <is>
-          <t>84</t>
-        </is>
+      <c r="A221" t="n">
+        <v>84</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
@@ -10379,12 +10601,13 @@
           <t>Central and South America</t>
         </is>
       </c>
+      <c r="J221" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="222">
-      <c r="A222" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
+      <c r="A222" t="n">
+        <v>85</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
@@ -10424,12 +10647,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J222" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
+      <c r="A223" t="n">
+        <v>85</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
@@ -10469,12 +10693,13 @@
           <t>China</t>
         </is>
       </c>
+      <c r="J223" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="224">
-      <c r="A224" t="inlineStr">
-        <is>
-          <t>86</t>
-        </is>
+      <c r="A224" t="n">
+        <v>86</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
@@ -10514,12 +10739,13 @@
           <t>Geneva, Switzerland</t>
         </is>
       </c>
+      <c r="J224" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="225">
-      <c r="A225" t="inlineStr">
-        <is>
-          <t>86</t>
-        </is>
+      <c r="A225" t="n">
+        <v>86</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
@@ -10559,12 +10785,13 @@
           <t>Burbank, California, USA</t>
         </is>
       </c>
+      <c r="J225" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>87</t>
-        </is>
+      <c r="A226" t="n">
+        <v>87</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
@@ -10604,12 +10831,13 @@
           <t>Pablo Picasso</t>
         </is>
       </c>
+      <c r="J226" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
-      <c r="A227" t="inlineStr">
-        <is>
-          <t>87</t>
-        </is>
+      <c r="A227" t="n">
+        <v>87</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
@@ -10649,12 +10877,13 @@
           <t>Miyazaki, Hayao</t>
         </is>
       </c>
+      <c r="J227" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="228">
-      <c r="A228" t="inlineStr">
-        <is>
-          <t>88</t>
-        </is>
+      <c r="A228" t="n">
+        <v>88</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
@@ -10694,12 +10923,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J228" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>88</t>
-        </is>
+      <c r="A229" t="n">
+        <v>88</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
@@ -10739,12 +10969,13 @@
           <t>Cyrillic</t>
         </is>
       </c>
+      <c r="J229" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="A230" t="n">
+        <v>89</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
@@ -10784,12 +11015,13 @@
           <t>2005</t>
         </is>
       </c>
+      <c r="J230" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="A231" t="n">
+        <v>89</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
@@ -10829,12 +11061,13 @@
           <t>2007</t>
         </is>
       </c>
+      <c r="J231" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="232">
-      <c r="A232" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="A232" t="n">
+        <v>89</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
@@ -10874,12 +11107,13 @@
           <t>1803 to 1815</t>
         </is>
       </c>
+      <c r="J232" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="233">
-      <c r="A233" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="A233" t="n">
+        <v>89</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
@@ -10919,12 +11153,13 @@
           <t>1651</t>
         </is>
       </c>
+      <c r="J233" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="234">
-      <c r="A234" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="A234" t="n">
+        <v>90</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
@@ -10964,12 +11199,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J234" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="A235" t="n">
+        <v>90</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
@@ -11009,12 +11245,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J235" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
+      <c r="A236" t="n">
+        <v>91</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
@@ -11054,12 +11291,13 @@
           <t>Australia</t>
         </is>
       </c>
+      <c r="J236" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
+      <c r="A237" t="n">
+        <v>91</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
@@ -11099,12 +11337,13 @@
           <t>Tropical and subtropical waters</t>
         </is>
       </c>
+      <c r="J237" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr">
-        <is>
-          <t>92</t>
-        </is>
+      <c r="A238" t="n">
+        <v>92</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
@@ -11144,12 +11383,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J238" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="239">
-      <c r="A239" t="inlineStr">
-        <is>
-          <t>92</t>
-        </is>
+      <c r="A239" t="n">
+        <v>92</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
@@ -11189,12 +11429,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J239" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="240">
-      <c r="A240" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
+      <c r="A240" t="n">
+        <v>93</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
@@ -11234,12 +11475,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J240" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="241">
-      <c r="A241" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
+      <c r="A241" t="n">
+        <v>93</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
@@ -11279,12 +11521,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J241" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="242">
-      <c r="A242" t="inlineStr">
-        <is>
-          <t>94</t>
-        </is>
+      <c r="A242" t="n">
+        <v>94</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
@@ -11324,12 +11567,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J242" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="243">
-      <c r="A243" t="inlineStr">
-        <is>
-          <t>94</t>
-        </is>
+      <c r="A243" t="n">
+        <v>94</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
@@ -11369,12 +11613,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J243" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="244">
-      <c r="A244" t="inlineStr">
-        <is>
-          <t>95</t>
-        </is>
+      <c r="A244" t="n">
+        <v>95</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
@@ -11414,12 +11659,13 @@
           <t>Christianity</t>
         </is>
       </c>
+      <c r="J244" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="245">
-      <c r="A245" t="inlineStr">
-        <is>
-          <t>95</t>
-        </is>
+      <c r="A245" t="n">
+        <v>95</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
@@ -11459,12 +11705,13 @@
           <t>Protestantism</t>
         </is>
       </c>
+      <c r="J245" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
+      <c r="A246" t="n">
+        <v>96</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
@@ -11504,12 +11751,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J246" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="247">
-      <c r="A247" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
+      <c r="A247" t="n">
+        <v>96</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
@@ -11549,12 +11797,13 @@
           <t>Latin alphabet</t>
         </is>
       </c>
+      <c r="J247" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="248">
-      <c r="A248" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
+      <c r="A248" t="n">
+        <v>97</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
@@ -11594,12 +11843,13 @@
           <t>North America</t>
         </is>
       </c>
+      <c r="J248" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
-      <c r="A249" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
+      <c r="A249" t="n">
+        <v>97</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
@@ -11639,12 +11889,13 @@
           <t>Northern, central, and eastern Africa</t>
         </is>
       </c>
+      <c r="J249" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="250">
-      <c r="A250" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
+      <c r="A250" t="n">
+        <v>98</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
@@ -11684,12 +11935,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J250" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="251">
-      <c r="A251" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
+      <c r="A251" t="n">
+        <v>98</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
@@ -11729,12 +11981,13 @@
           <t>Roman Catholicism</t>
         </is>
       </c>
+      <c r="J251" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="252">
-      <c r="A252" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+      <c r="A252" t="n">
+        <v>99</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
@@ -11774,12 +12027,13 @@
           <t>Pablo Picasso</t>
         </is>
       </c>
+      <c r="J252" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
-      <c r="A253" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+      <c r="A253" t="n">
+        <v>99</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
@@ -11818,6 +12072,9 @@
         <is>
           <t>Asghar Farhadi</t>
         </is>
+      </c>
+      <c r="J253" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>